<commit_message>
ke: sch sth update forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Kenya/ke_sch_sth_sppm_202403_1_wash.xlsx
+++ b/SCH-STH/Impact assessments/Kenya/ke_sch_sth_sppm_202403_1_wash.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Kenya\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7928672-8486-4FF5-BC92-194C9CE5FE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7411C3-2D01-4548-A6FA-89ECDA989E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7722" uniqueCount="1095">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7724" uniqueCount="1095">
   <si>
     <t>type</t>
   </si>
@@ -3926,7 +3926,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19:H20"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4337,11 +4337,14 @@
       <c r="B21" t="s">
         <v>360</v>
       </c>
+      <c r="H21" s="7" t="s">
+        <v>1079</v>
+      </c>
       <c r="I21" s="7" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -4356,6 +4359,9 @@
       </c>
       <c r="G22" s="14" t="s">
         <v>370</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>1079</v>
       </c>
       <c r="I22" s="7" t="s">
         <v>363</v>
@@ -4694,7 +4700,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>8</v>
       </c>
@@ -4848,7 +4854,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>8</v>
       </c>
@@ -4874,7 +4880,7 @@
       <c r="K49" s="11"/>
       <c r="L49" s="11"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>306</v>
       </c>
@@ -4965,7 +4971,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>358</v>
       </c>
@@ -36949,15 +36955,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F61D857ACC8084D9287671D8B7E15F4" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0c3a67db788bfb057b2db4972c06362d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="92042fd9-f4c9-49ed-97f1-ba485e322b1e" xmlns:ns3="744cc826-a471-4feb-879c-6424ce8a761f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="13059b5e6b4741244ec9ec4e04bff113" ns2:_="" ns3:_="">
     <xsd:import namespace="92042fd9-f4c9-49ed-97f1-ba485e322b1e"/>
@@ -37192,15 +37189,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFA7685D-B04F-4991-951F-5668DE28AE41}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D52A5182-A145-49DC-8B93-E3BAA13C11F0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37217,4 +37215,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFA7685D-B04F-4991-951F-5668DE28AE41}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>